<commit_message>
Add generated schedule data files
</commit_message>
<xml_diff>
--- a/py_version/src/schedules/schedule.xlsx
+++ b/py_version/src/schedules/schedule.xlsx
@@ -490,10 +490,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -527,10 +525,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -564,10 +560,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -601,10 +595,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -638,10 +630,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -675,10 +665,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A7" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -712,10 +700,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="A8" t="n">
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -749,10 +735,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="A9" t="n">
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -786,10 +770,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="A10" t="n">
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -879,10 +861,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -919,10 +899,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -959,10 +937,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -998,10 +974,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -1036,10 +1010,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -1076,10 +1048,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A7" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -1115,10 +1085,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="A8" t="n">
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -1154,10 +1122,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="A9" t="n">
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1193,10 +1159,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="A10" t="n">
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1288,10 +1252,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -1328,10 +1290,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -1369,10 +1329,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -1408,10 +1366,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -1447,10 +1403,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -1485,10 +1439,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A7" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -1523,10 +1475,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="A8" t="n">
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -1560,10 +1510,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="A9" t="n">
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1597,10 +1545,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="A10" t="n">
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1690,10 +1636,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -1727,10 +1671,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -1766,10 +1708,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -1804,10 +1744,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -1842,10 +1780,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -1880,10 +1816,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A7" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -1918,10 +1852,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="A8" t="n">
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -1955,10 +1887,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="A9" t="n">
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1992,10 +1922,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="A10" t="n">
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -2085,10 +2013,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -2123,10 +2049,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -2161,10 +2085,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -2198,10 +2120,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -2235,10 +2155,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -2272,10 +2190,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A7" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -2311,10 +2227,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="A8" t="n">
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -2351,10 +2265,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="A9" t="n">
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -2390,10 +2302,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="A10" t="n">
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -2483,10 +2393,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -2524,10 +2432,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -2565,10 +2471,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -2606,10 +2510,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -2646,10 +2548,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -2684,10 +2584,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A7" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -2722,10 +2620,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="A8" t="n">
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -2760,10 +2656,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="A9" t="n">
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -2797,10 +2691,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="A10" t="n">
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -2890,10 +2782,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -2927,10 +2817,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -2966,10 +2854,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -3005,10 +2891,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -3043,10 +2927,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -3080,10 +2962,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A7" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -3117,10 +2997,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="A8" t="n">
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -3210,10 +3088,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -3247,10 +3123,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -3284,10 +3158,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -3321,10 +3193,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -3359,10 +3229,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -3397,10 +3265,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A7" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -3435,10 +3301,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="A8" t="n">
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -3472,10 +3336,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="A9" t="n">
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -3510,10 +3372,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="A10" t="n">
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -3603,10 +3463,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -3640,10 +3498,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -3677,10 +3533,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -3714,10 +3568,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -3752,10 +3604,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -3790,10 +3640,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A7" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -3827,10 +3675,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="A8" t="n">
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -3864,10 +3710,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="A9" t="n">
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -3957,10 +3801,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -3994,10 +3836,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -4031,10 +3871,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -4068,10 +3906,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -4105,10 +3941,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -4142,10 +3976,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A7" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -4180,10 +4012,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="A8" t="n">
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -4217,10 +4047,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="A9" t="n">
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -4311,10 +4139,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -4348,10 +4174,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -4441,10 +4265,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -4483,10 +4305,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -4524,10 +4344,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -4566,10 +4384,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -4606,10 +4422,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -4646,10 +4460,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A7" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -4685,10 +4497,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="A8" t="n">
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -4723,10 +4533,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="A9" t="n">
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -4761,10 +4569,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="A10" t="n">
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -4798,10 +4604,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+      <c r="A11" t="n">
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -4891,10 +4695,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -4928,10 +4730,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -4965,10 +4765,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -5002,10 +4800,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -5039,10 +4835,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -5076,10 +4870,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A7" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -5113,10 +4905,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="A8" t="n">
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -5206,10 +4996,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -5243,10 +5031,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -5281,10 +5067,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -5320,10 +5104,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -5358,10 +5140,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -5399,10 +5179,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A7" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -5440,10 +5218,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="A8" t="n">
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -5481,10 +5257,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="A9" t="n">
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -5521,10 +5295,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="A10" t="n">
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -5615,10 +5387,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -5652,10 +5422,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -5690,10 +5458,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -5730,10 +5496,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -5771,10 +5535,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -5813,10 +5575,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A7" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -5853,10 +5613,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="A8" t="n">
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -5891,10 +5649,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="A9" t="n">
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -5929,10 +5685,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="A10" t="n">
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -6022,10 +5776,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -6060,10 +5812,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -6099,10 +5849,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -6138,10 +5886,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -6177,10 +5923,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -6216,10 +5960,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A7" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -6257,10 +5999,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="A8" t="n">
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -6297,10 +6037,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="A9" t="n">
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -6336,10 +6074,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="A10" t="n">
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -6429,10 +6165,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -6467,10 +6201,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -6505,10 +6237,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -6544,10 +6274,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -6584,10 +6312,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -6626,10 +6352,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A7" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -6666,10 +6390,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="A8" t="n">
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -6706,10 +6428,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="A9" t="n">
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -6800,10 +6520,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -6838,10 +6556,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -6876,10 +6592,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -6915,10 +6629,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -6954,10 +6666,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -6991,10 +6701,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A7" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -7029,10 +6737,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="A8" t="n">
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -7066,10 +6772,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="A9" t="n">
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -7104,10 +6808,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="A10" t="n">
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -7142,10 +6844,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+      <c r="A11" t="n">
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -7180,10 +6880,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="A12" t="n">
+        <v>11</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -7217,10 +6915,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+      <c r="A13" t="n">
+        <v>12</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -7310,10 +7006,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -7348,10 +7042,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -7386,10 +7078,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -7425,10 +7115,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -7465,10 +7153,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -7503,10 +7189,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A7" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -7542,10 +7226,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="A8" t="n">
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -7581,10 +7263,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="A9" t="n">
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -7619,10 +7299,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="A10" t="n">
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -7658,10 +7336,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+      <c r="A11" t="n">
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -7696,10 +7372,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="A12" t="n">
+        <v>11</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -7733,10 +7407,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+      <c r="A13" t="n">
+        <v>12</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -7826,10 +7498,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -7865,10 +7535,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -7904,10 +7572,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -7945,10 +7611,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -7985,10 +7649,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -8026,10 +7688,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A7" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -8068,10 +7728,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="A8" t="n">
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -8107,10 +7765,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="A9" t="n">
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -8146,10 +7802,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="A10" t="n">
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -8183,10 +7837,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+      <c r="A11" t="n">
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -8220,10 +7872,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="A12" t="n">
+        <v>11</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update schedule files, add new schedule-teachers.xlsx
</commit_message>
<xml_diff>
--- a/py_version/src/schedules/schedule.xlsx
+++ b/py_version/src/schedules/schedule.xlsx
@@ -1626,7 +1626,11 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n"/>
-      <c r="B5" s="2" t="n"/>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>8:00-8:45</t>
+        </is>
+      </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
           <t>pr.k.p.fry-fry</t>
@@ -1756,7 +1760,11 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n"/>
-      <c r="B7" s="2" t="n"/>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>8:50-9:35</t>
+        </is>
+      </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
           <t>pr.k.p.fry-fry</t>
@@ -1882,7 +1890,11 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n"/>
-      <c r="B9" s="2" t="n"/>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>9:40-10:25</t>
+        </is>
+      </c>
       <c r="C9" s="1" t="inlineStr"/>
       <c r="D9" s="1" t="inlineStr"/>
       <c r="E9" s="1" t="inlineStr"/>
@@ -1996,7 +2008,11 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n"/>
-      <c r="B11" s="2" t="n"/>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>10:40-11:25</t>
+        </is>
+      </c>
       <c r="C11" s="1" t="inlineStr"/>
       <c r="D11" s="1" t="inlineStr"/>
       <c r="E11" s="1" t="inlineStr"/>
@@ -2104,7 +2120,11 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n"/>
-      <c r="B13" s="2" t="n"/>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>11:30-12:15</t>
+        </is>
+      </c>
       <c r="C13" s="1" t="inlineStr">
         <is>
           <t>p.i.d.fry-fry</t>
@@ -2234,7 +2254,11 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n"/>
-      <c r="B15" s="2" t="n"/>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>12:20-13:05</t>
+        </is>
+      </c>
       <c r="C15" s="1" t="inlineStr">
         <is>
           <t>p.i.d.fry-fry</t>
@@ -2344,7 +2368,11 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n"/>
-      <c r="B17" s="2" t="n"/>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>13:10-13:55</t>
+        </is>
+      </c>
       <c r="C17" s="1" t="inlineStr"/>
       <c r="D17" s="1" t="inlineStr"/>
       <c r="E17" s="1" t="inlineStr"/>
@@ -2442,7 +2470,11 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n"/>
-      <c r="B19" s="2" t="n"/>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>14:10-14:55</t>
+        </is>
+      </c>
       <c r="C19" s="1" t="inlineStr"/>
       <c r="D19" s="1" t="inlineStr"/>
       <c r="E19" s="1" t="inlineStr"/>
@@ -2542,7 +2574,11 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n"/>
-      <c r="B21" s="2" t="n"/>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>15:00-15:45</t>
+        </is>
+      </c>
       <c r="C21" s="1" t="inlineStr"/>
       <c r="D21" s="1" t="inlineStr"/>
       <c r="E21" s="1" t="inlineStr"/>
@@ -2582,30 +2618,21 @@
       <c r="Q21" s="1" t="inlineStr"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="14">
+    <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="A20:A21"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B16:B17"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2868,7 +2895,11 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n"/>
-      <c r="B5" s="2" t="n"/>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>8:00-8:45</t>
+        </is>
+      </c>
       <c r="C5" s="1" t="inlineStr"/>
       <c r="D5" s="1" t="inlineStr"/>
       <c r="E5" s="1" t="inlineStr"/>
@@ -2994,7 +3025,11 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n"/>
-      <c r="B7" s="2" t="n"/>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>8:50-9:35</t>
+        </is>
+      </c>
       <c r="C7" s="1" t="inlineStr"/>
       <c r="D7" s="1" t="inlineStr"/>
       <c r="E7" s="1" t="inlineStr"/>
@@ -3128,7 +3163,11 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n"/>
-      <c r="B9" s="2" t="n"/>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>9:40-10:25</t>
+        </is>
+      </c>
       <c r="C9" s="1" t="inlineStr"/>
       <c r="D9" s="1" t="inlineStr"/>
       <c r="E9" s="1" t="inlineStr"/>
@@ -3244,7 +3283,11 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n"/>
-      <c r="B11" s="2" t="n"/>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>10:40-11:25</t>
+        </is>
+      </c>
       <c r="C11" s="1" t="inlineStr"/>
       <c r="D11" s="1" t="inlineStr"/>
       <c r="E11" s="1" t="inlineStr"/>
@@ -3360,7 +3403,11 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n"/>
-      <c r="B13" s="2" t="n"/>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>11:30-12:15</t>
+        </is>
+      </c>
       <c r="C13" s="1" t="inlineStr"/>
       <c r="D13" s="1" t="inlineStr"/>
       <c r="E13" s="1" t="inlineStr"/>
@@ -3466,7 +3513,11 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n"/>
-      <c r="B15" s="2" t="n"/>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>12:20-13:05</t>
+        </is>
+      </c>
       <c r="C15" s="1" t="inlineStr"/>
       <c r="D15" s="1" t="inlineStr"/>
       <c r="E15" s="1" t="inlineStr"/>
@@ -3673,23 +3724,17 @@
       <c r="Q18" s="1" t="inlineStr"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="11">
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="O1:Q1"/>
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B4:B5"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B12:B13"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:K1"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B10:B11"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B6:B7"/>
     <mergeCell ref="A14:A15"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4032,7 +4077,11 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n"/>
-      <c r="B6" s="2" t="n"/>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>8:50-9:35</t>
+        </is>
+      </c>
       <c r="C6" s="1" t="inlineStr"/>
       <c r="D6" s="1" t="inlineStr"/>
       <c r="E6" s="1" t="inlineStr"/>
@@ -4148,7 +4197,11 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n"/>
-      <c r="B8" s="2" t="n"/>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>9:40-10:25</t>
+        </is>
+      </c>
       <c r="C8" s="1" t="inlineStr"/>
       <c r="D8" s="1" t="inlineStr"/>
       <c r="E8" s="1" t="inlineStr"/>
@@ -4252,7 +4305,11 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n"/>
-      <c r="B10" s="2" t="n"/>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>10:40-11:25</t>
+        </is>
+      </c>
       <c r="C10" s="1" t="inlineStr"/>
       <c r="D10" s="1" t="inlineStr"/>
       <c r="E10" s="1" t="inlineStr"/>
@@ -4358,7 +4415,11 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n"/>
-      <c r="B12" s="2" t="n"/>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>11:30-12:15</t>
+        </is>
+      </c>
       <c r="C12" s="1" t="inlineStr"/>
       <c r="D12" s="1" t="inlineStr"/>
       <c r="E12" s="1" t="inlineStr"/>
@@ -4464,7 +4525,11 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n"/>
-      <c r="B14" s="2" t="n"/>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>12:20-13:05</t>
+        </is>
+      </c>
       <c r="C14" s="1" t="inlineStr"/>
       <c r="D14" s="1" t="inlineStr"/>
       <c r="E14" s="1" t="inlineStr"/>
@@ -4659,21 +4724,16 @@
       <c r="Q17" s="1" t="inlineStr"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="10">
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="B9:B10"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B5:B6"/>
     <mergeCell ref="A11:A12"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4935,7 +4995,11 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n"/>
-      <c r="B5" s="2" t="n"/>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>8:00-8:45</t>
+        </is>
+      </c>
       <c r="C5" s="1" t="inlineStr"/>
       <c r="D5" s="1" t="inlineStr"/>
       <c r="E5" s="1" t="inlineStr"/>
@@ -5041,7 +5105,11 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n"/>
-      <c r="B7" s="2" t="n"/>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>8:50-9:35</t>
+        </is>
+      </c>
       <c r="C7" s="1" t="inlineStr"/>
       <c r="D7" s="1" t="inlineStr"/>
       <c r="E7" s="1" t="inlineStr"/>
@@ -5382,7 +5450,11 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n"/>
-      <c r="B12" s="2" t="n"/>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>12:20-13:05</t>
+        </is>
+      </c>
       <c r="C12" s="1" t="inlineStr"/>
       <c r="D12" s="1" t="inlineStr"/>
       <c r="E12" s="1" t="inlineStr"/>
@@ -5500,7 +5572,11 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n"/>
-      <c r="B14" s="2" t="n"/>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>13:10-13:55</t>
+        </is>
+      </c>
       <c r="C14" s="1" t="inlineStr">
         <is>
           <t>p.i.w.zap-log</t>
@@ -5626,7 +5702,11 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="n"/>
-      <c r="B16" s="2" t="n"/>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>14:10-14:55</t>
+        </is>
+      </c>
       <c r="C16" s="1" t="inlineStr">
         <is>
           <t>p.i.w.zap-log</t>
@@ -5701,22 +5781,17 @@
       <c r="Q17" s="1" t="inlineStr"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="10">
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="B4:B5"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B11:B12"/>
     <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
     <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B15:B16"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -5981,7 +6056,11 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n"/>
-      <c r="B5" s="2" t="n"/>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>8:00-8:45</t>
+        </is>
+      </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
           <t>wło-log</t>
@@ -6119,7 +6198,11 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n"/>
-      <c r="B7" s="2" t="n"/>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>8:50-9:35</t>
+        </is>
+      </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
           <t>infor-log</t>
@@ -6259,7 +6342,11 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n"/>
-      <c r="B9" s="2" t="n"/>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>9:40-10:25</t>
+        </is>
+      </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
           <t>przech.zap-log</t>
@@ -6401,7 +6488,11 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n"/>
-      <c r="B11" s="2" t="n"/>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>10:40-11:25</t>
+        </is>
+      </c>
       <c r="C11" s="1" t="inlineStr">
         <is>
           <t>przech.zap-log</t>
@@ -6531,7 +6622,11 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n"/>
-      <c r="B13" s="2" t="n"/>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>11:30-12:15</t>
+        </is>
+      </c>
       <c r="C13" s="1" t="inlineStr">
         <is>
           <t>w.f-log</t>
@@ -6639,7 +6734,11 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n"/>
-      <c r="B15" s="2" t="n"/>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>12:20-13:05</t>
+        </is>
+      </c>
       <c r="C15" s="1" t="inlineStr">
         <is>
           <t>w.f-log</t>
@@ -6745,7 +6844,11 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n"/>
-      <c r="B17" s="2" t="n"/>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>13:10-13:55</t>
+        </is>
+      </c>
       <c r="C17" s="1" t="inlineStr"/>
       <c r="D17" s="1" t="inlineStr"/>
       <c r="E17" s="1" t="inlineStr"/>
@@ -6855,26 +6958,19 @@
       <c r="Q19" s="1" t="inlineStr"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="12">
+    <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B16:B17"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -7174,7 +7270,11 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n"/>
-      <c r="B6" s="2" t="n"/>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>8:50-9:35</t>
+        </is>
+      </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
           <t>ang-j2</t>
@@ -7270,7 +7370,11 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n"/>
-      <c r="B8" s="2" t="n"/>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>9:40-10:25</t>
+        </is>
+      </c>
       <c r="C8" s="1" t="inlineStr">
         <is>
           <t>w.f-j2</t>
@@ -7370,7 +7474,11 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n"/>
-      <c r="B10" s="2" t="n"/>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>10:40-11:25</t>
+        </is>
+      </c>
       <c r="C10" s="1" t="inlineStr"/>
       <c r="D10" s="1" t="inlineStr"/>
       <c r="E10" s="1" t="inlineStr"/>
@@ -7553,18 +7661,15 @@
       <c r="Q13" s="1" t="inlineStr"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="8">
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="B9:B10"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -7932,7 +8037,11 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n"/>
-      <c r="B8" s="2" t="n"/>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>10:40-11:25</t>
+        </is>
+      </c>
       <c r="C8" s="1" t="inlineStr"/>
       <c r="D8" s="1" t="inlineStr"/>
       <c r="E8" s="1" t="inlineStr"/>
@@ -8008,7 +8117,11 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n"/>
-      <c r="B10" s="2" t="n"/>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>11:30-12:15</t>
+        </is>
+      </c>
       <c r="C10" s="1" t="inlineStr"/>
       <c r="D10" s="1" t="inlineStr"/>
       <c r="E10" s="1" t="inlineStr"/>
@@ -8084,7 +8197,11 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n"/>
-      <c r="B12" s="2" t="n"/>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>12:20-13:05</t>
+        </is>
+      </c>
       <c r="C12" s="1" t="inlineStr"/>
       <c r="D12" s="1" t="inlineStr"/>
       <c r="E12" s="1" t="inlineStr"/>
@@ -8199,7 +8316,11 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n"/>
-      <c r="B15" s="2" t="n"/>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>14:10-14:55</t>
+        </is>
+      </c>
       <c r="C15" s="1" t="inlineStr"/>
       <c r="D15" s="1" t="inlineStr"/>
       <c r="E15" s="1" t="inlineStr"/>
@@ -8264,19 +8385,15 @@
       <c r="Q16" s="1" t="inlineStr"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="9">
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="B9:B10"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B14:B15"/>
     <mergeCell ref="A11:A12"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8649,7 +8766,11 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n"/>
-      <c r="B8" s="2" t="n"/>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>10:40-11:25</t>
+        </is>
+      </c>
       <c r="C8" s="1" t="inlineStr"/>
       <c r="D8" s="1" t="inlineStr"/>
       <c r="E8" s="1" t="inlineStr"/>
@@ -8723,7 +8844,11 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n"/>
-      <c r="B10" s="2" t="n"/>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>11:30-12:15</t>
+        </is>
+      </c>
       <c r="C10" s="1" t="inlineStr"/>
       <c r="D10" s="1" t="inlineStr"/>
       <c r="E10" s="1" t="inlineStr"/>
@@ -8882,16 +9007,14 @@
       <c r="Q13" s="1" t="inlineStr"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="7">
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="B9:B10"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -9343,7 +9466,11 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n"/>
-      <c r="B10" s="2" t="n"/>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>12:20-13:05</t>
+        </is>
+      </c>
       <c r="C10" s="1" t="inlineStr"/>
       <c r="D10" s="1" t="inlineStr"/>
       <c r="E10" s="1" t="inlineStr"/>
@@ -9466,7 +9593,11 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n"/>
-      <c r="B13" s="2" t="n"/>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>14:10-14:55</t>
+        </is>
+      </c>
       <c r="C13" s="1" t="inlineStr"/>
       <c r="D13" s="1" t="inlineStr"/>
       <c r="E13" s="1" t="inlineStr"/>
@@ -9496,14 +9627,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="7">
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="B9:B10"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:K1"/>
   </mergeCells>
@@ -10026,7 +10155,11 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n"/>
-      <c r="B5" s="2" t="n"/>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>8:00-8:45</t>
+        </is>
+      </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
           <t>pr.fry.men-fry</t>
@@ -10178,7 +10311,11 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n"/>
-      <c r="B7" s="2" t="n"/>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>8:50-9:35</t>
+        </is>
+      </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
           <t>pr.fry.men-fry</t>
@@ -10318,7 +10455,11 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n"/>
-      <c r="B9" s="2" t="n"/>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>9:40-10:25</t>
+        </is>
+      </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
           <t>pr.est-fry</t>
@@ -10466,7 +10607,11 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n"/>
-      <c r="B11" s="2" t="n"/>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>10:40-11:25</t>
+        </is>
+      </c>
       <c r="C11" s="1" t="inlineStr">
         <is>
           <t>p.i.d.fry-fry</t>
@@ -10594,7 +10739,11 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n"/>
-      <c r="B13" s="2" t="n"/>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>11:30-12:15</t>
+        </is>
+      </c>
       <c r="C13" s="1" t="inlineStr">
         <is>
           <t>pod.fry-fry</t>
@@ -10720,7 +10869,11 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n"/>
-      <c r="B15" s="2" t="n"/>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>12:20-13:05</t>
+        </is>
+      </c>
       <c r="C15" s="1" t="inlineStr">
         <is>
           <t>t.fry-fry</t>
@@ -10836,7 +10989,11 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n"/>
-      <c r="B17" s="2" t="n"/>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>13:10-13:55</t>
+        </is>
+      </c>
       <c r="C17" s="1" t="inlineStr">
         <is>
           <t>pr.fry.dam-fry</t>
@@ -10944,7 +11101,11 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n"/>
-      <c r="B19" s="2" t="n"/>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>14:10-14:55</t>
+        </is>
+      </c>
       <c r="C19" s="1" t="inlineStr">
         <is>
           <t>pr.fry.dam-fry</t>
@@ -11092,28 +11253,20 @@
       <c r="Q21" s="1" t="inlineStr"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="13">
+    <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B16:B17"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -11990,7 +12143,11 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n"/>
-      <c r="B6" s="2" t="n"/>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>8:50-9:35</t>
+        </is>
+      </c>
       <c r="C6" s="1" t="inlineStr"/>
       <c r="D6" s="1" t="inlineStr"/>
       <c r="E6" s="1" t="inlineStr"/>
@@ -12098,7 +12255,11 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n"/>
-      <c r="B8" s="2" t="n"/>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>9:40-10:25</t>
+        </is>
+      </c>
       <c r="C8" s="1" t="inlineStr"/>
       <c r="D8" s="1" t="inlineStr"/>
       <c r="E8" s="1" t="inlineStr"/>
@@ -12212,7 +12373,11 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n"/>
-      <c r="B10" s="2" t="n"/>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>10:40-11:25</t>
+        </is>
+      </c>
       <c r="C10" s="1" t="inlineStr"/>
       <c r="D10" s="1" t="inlineStr"/>
       <c r="E10" s="1" t="inlineStr"/>
@@ -12316,7 +12481,11 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n"/>
-      <c r="B12" s="2" t="n"/>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>11:30-12:15</t>
+        </is>
+      </c>
       <c r="C12" s="1" t="inlineStr"/>
       <c r="D12" s="1" t="inlineStr"/>
       <c r="E12" s="1" t="inlineStr"/>
@@ -12369,7 +12538,11 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n"/>
-      <c r="B13" s="2" t="n"/>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>11:30-12:15</t>
+        </is>
+      </c>
       <c r="C13" s="1" t="inlineStr"/>
       <c r="D13" s="1" t="inlineStr"/>
       <c r="E13" s="1" t="inlineStr"/>
@@ -12475,7 +12648,11 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n"/>
-      <c r="B15" s="2" t="n"/>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>12:20-13:05</t>
+        </is>
+      </c>
       <c r="C15" s="1" t="inlineStr"/>
       <c r="D15" s="1" t="inlineStr"/>
       <c r="E15" s="1" t="inlineStr"/>
@@ -12528,7 +12705,11 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="n"/>
-      <c r="B16" s="2" t="n"/>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>12:20-13:05</t>
+        </is>
+      </c>
       <c r="C16" s="1" t="inlineStr"/>
       <c r="D16" s="1" t="inlineStr"/>
       <c r="E16" s="1" t="inlineStr"/>
@@ -12636,7 +12817,11 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="n"/>
-      <c r="B18" s="2" t="n"/>
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>13:10-13:55</t>
+        </is>
+      </c>
       <c r="C18" s="1" t="inlineStr"/>
       <c r="D18" s="1" t="inlineStr"/>
       <c r="E18" s="1" t="inlineStr"/>
@@ -12689,7 +12874,11 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n"/>
-      <c r="B19" s="2" t="n"/>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>13:10-13:55</t>
+        </is>
+      </c>
       <c r="C19" s="1" t="inlineStr"/>
       <c r="D19" s="1" t="inlineStr"/>
       <c r="E19" s="1" t="inlineStr"/>
@@ -12787,7 +12976,11 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n"/>
-      <c r="B21" s="2" t="n"/>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>14:10-14:55</t>
+        </is>
+      </c>
       <c r="C21" s="1" t="inlineStr"/>
       <c r="D21" s="1" t="inlineStr"/>
       <c r="E21" s="1" t="inlineStr"/>
@@ -12828,7 +13021,11 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="n"/>
-      <c r="B22" s="2" t="n"/>
+      <c r="B22" s="2" t="inlineStr">
+        <is>
+          <t>14:10-14:55</t>
+        </is>
+      </c>
       <c r="C22" s="1" t="inlineStr"/>
       <c r="D22" s="1" t="inlineStr"/>
       <c r="E22" s="1" t="inlineStr"/>
@@ -12904,7 +13101,11 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="n"/>
-      <c r="B24" s="2" t="n"/>
+      <c r="B24" s="2" t="inlineStr">
+        <is>
+          <t>15:00-15:45</t>
+        </is>
+      </c>
       <c r="C24" s="1" t="inlineStr"/>
       <c r="D24" s="1" t="inlineStr"/>
       <c r="E24" s="1" t="inlineStr"/>
@@ -12934,28 +13135,20 @@
       <c r="Q24" s="1" t="inlineStr"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="13">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="A9:A10"/>
     <mergeCell ref="A17:A19"/>
+    <mergeCell ref="F1:H1"/>
     <mergeCell ref="A20:A22"/>
+    <mergeCell ref="I1:K1"/>
     <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="F1:H1"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A14:A16"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -13291,7 +13484,11 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n"/>
-      <c r="B6" s="2" t="n"/>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>8:50-9:35</t>
+        </is>
+      </c>
       <c r="C6" s="1" t="inlineStr"/>
       <c r="D6" s="1" t="inlineStr"/>
       <c r="E6" s="1" t="inlineStr"/>
@@ -13395,7 +13592,11 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n"/>
-      <c r="B8" s="2" t="n"/>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>9:40-10:25</t>
+        </is>
+      </c>
       <c r="C8" s="1" t="inlineStr"/>
       <c r="D8" s="1" t="inlineStr"/>
       <c r="E8" s="1" t="inlineStr"/>
@@ -13521,7 +13722,11 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n"/>
-      <c r="B10" s="2" t="n"/>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>10:40-11:25</t>
+        </is>
+      </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
           <t>dok.r.pr.tr-log</t>
@@ -13665,7 +13870,11 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n"/>
-      <c r="B12" s="2" t="n"/>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>11:30-12:15</t>
+        </is>
+      </c>
       <c r="C12" s="1" t="inlineStr">
         <is>
           <t>dok.r.pr.tr-log</t>
@@ -13815,7 +14024,11 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n"/>
-      <c r="B14" s="2" t="n"/>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>12:20-13:05</t>
+        </is>
+      </c>
       <c r="C14" s="1" t="inlineStr">
         <is>
           <t>dok.r.pr.tr-log</t>
@@ -13941,7 +14154,11 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="n"/>
-      <c r="B16" s="2" t="n"/>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>13:10-13:55</t>
+        </is>
+      </c>
       <c r="C16" s="1" t="inlineStr"/>
       <c r="D16" s="1" t="inlineStr"/>
       <c r="E16" s="1" t="inlineStr"/>
@@ -14035,7 +14252,11 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="n"/>
-      <c r="B18" s="2" t="n"/>
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>14:10-14:55</t>
+        </is>
+      </c>
       <c r="C18" s="1" t="inlineStr"/>
       <c r="D18" s="1" t="inlineStr"/>
       <c r="E18" s="1" t="inlineStr"/>
@@ -14098,25 +14319,18 @@
       <c r="Q19" s="1" t="inlineStr"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="12">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B9:B10"/>
     <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A9:A10"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="F1:H1"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="I1:K1"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A7:A8"/>
     <mergeCell ref="A11:A12"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -14380,7 +14594,11 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n"/>
-      <c r="B5" s="2" t="n"/>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>8:00-8:45</t>
+        </is>
+      </c>
       <c r="C5" s="1" t="inlineStr"/>
       <c r="D5" s="1" t="inlineStr"/>
       <c r="E5" s="1" t="inlineStr"/>
@@ -14488,7 +14706,11 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n"/>
-      <c r="B7" s="2" t="n"/>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>8:50-9:35</t>
+        </is>
+      </c>
       <c r="C7" s="1" t="inlineStr"/>
       <c r="D7" s="1" t="inlineStr"/>
       <c r="E7" s="1" t="inlineStr"/>
@@ -14606,7 +14828,11 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n"/>
-      <c r="B9" s="2" t="n"/>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>9:40-10:25</t>
+        </is>
+      </c>
       <c r="C9" s="1" t="inlineStr"/>
       <c r="D9" s="1" t="inlineStr"/>
       <c r="E9" s="1" t="inlineStr"/>
@@ -14722,7 +14948,11 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n"/>
-      <c r="B11" s="2" t="n"/>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>10:40-11:25</t>
+        </is>
+      </c>
       <c r="C11" s="1" t="inlineStr"/>
       <c r="D11" s="1" t="inlineStr"/>
       <c r="E11" s="1" t="inlineStr"/>
@@ -14838,7 +15068,11 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n"/>
-      <c r="B13" s="2" t="n"/>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>11:30-12:15</t>
+        </is>
+      </c>
       <c r="C13" s="1" t="inlineStr"/>
       <c r="D13" s="1" t="inlineStr"/>
       <c r="E13" s="1" t="inlineStr"/>
@@ -14956,7 +15190,11 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n"/>
-      <c r="B15" s="2" t="n"/>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>12:20-13:05</t>
+        </is>
+      </c>
       <c r="C15" s="1" t="inlineStr">
         <is>
           <t>ang-log</t>
@@ -15082,7 +15320,11 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n"/>
-      <c r="B17" s="2" t="n"/>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>13:10-13:55</t>
+        </is>
+      </c>
       <c r="C17" s="1" t="inlineStr">
         <is>
           <t>pl.p.trans-log</t>
@@ -15178,7 +15420,11 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n"/>
-      <c r="B19" s="2" t="n"/>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>14:10-14:55</t>
+        </is>
+      </c>
       <c r="C19" s="1" t="inlineStr">
         <is>
           <t>pl.p.trans-log</t>
@@ -15261,28 +15507,20 @@
       <c r="Q20" s="1" t="inlineStr"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="13">
+    <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B16:B17"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -15543,7 +15781,11 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n"/>
-      <c r="B5" s="2" t="n"/>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>8:00-8:45</t>
+        </is>
+      </c>
       <c r="C5" s="1" t="inlineStr"/>
       <c r="D5" s="1" t="inlineStr"/>
       <c r="E5" s="1" t="inlineStr"/>
@@ -15647,7 +15889,11 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n"/>
-      <c r="B7" s="2" t="n"/>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>8:50-9:35</t>
+        </is>
+      </c>
       <c r="C7" s="1" t="inlineStr"/>
       <c r="D7" s="1" t="inlineStr"/>
       <c r="E7" s="1" t="inlineStr"/>
@@ -15751,7 +15997,11 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n"/>
-      <c r="B9" s="2" t="n"/>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>9:40-10:25</t>
+        </is>
+      </c>
       <c r="C9" s="1" t="inlineStr"/>
       <c r="D9" s="1" t="inlineStr"/>
       <c r="E9" s="1" t="inlineStr"/>
@@ -15869,7 +16119,11 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n"/>
-      <c r="B11" s="2" t="n"/>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>10:40-11:25</t>
+        </is>
+      </c>
       <c r="C11" s="1" t="inlineStr">
         <is>
           <t>niem-log</t>
@@ -15999,7 +16253,11 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n"/>
-      <c r="B13" s="2" t="n"/>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>11:30-12:15</t>
+        </is>
+      </c>
       <c r="C13" s="1" t="inlineStr">
         <is>
           <t>o.m.z-log</t>
@@ -16149,7 +16407,11 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n"/>
-      <c r="B15" s="2" t="n"/>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>12:20-13:05</t>
+        </is>
+      </c>
       <c r="C15" s="1" t="inlineStr">
         <is>
           <t>k.p.s-log</t>
@@ -16281,7 +16543,11 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n"/>
-      <c r="B17" s="2" t="n"/>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>13:10-13:55</t>
+        </is>
+      </c>
       <c r="C17" s="1" t="inlineStr">
         <is>
           <t>w.f-log</t>
@@ -16415,7 +16681,11 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n"/>
-      <c r="B19" s="2" t="n"/>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>14:10-14:55</t>
+        </is>
+      </c>
       <c r="C19" s="1" t="inlineStr">
         <is>
           <t>w.f-log</t>
@@ -16445,28 +16715,20 @@
       <c r="Q19" s="1" t="inlineStr"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="13">
+    <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B16:B17"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -16735,7 +16997,11 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n"/>
-      <c r="B5" s="2" t="n"/>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>8:00-8:45</t>
+        </is>
+      </c>
       <c r="C5" s="1" t="inlineStr"/>
       <c r="D5" s="1" t="inlineStr"/>
       <c r="E5" s="1" t="inlineStr"/>
@@ -16847,7 +17113,11 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n"/>
-      <c r="B7" s="2" t="n"/>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>8:50-9:35</t>
+        </is>
+      </c>
       <c r="C7" s="1" t="inlineStr"/>
       <c r="D7" s="1" t="inlineStr"/>
       <c r="E7" s="1" t="inlineStr"/>
@@ -16955,7 +17225,11 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n"/>
-      <c r="B9" s="2" t="n"/>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>9:40-10:25</t>
+        </is>
+      </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
           <t>infor-j2</t>
@@ -17075,7 +17349,11 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n"/>
-      <c r="B11" s="2" t="n"/>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>10:40-11:25</t>
+        </is>
+      </c>
       <c r="C11" s="1" t="inlineStr">
         <is>
           <t>w.f-j2</t>
@@ -17270,7 +17548,11 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n"/>
-      <c r="B14" s="2" t="n"/>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>12:20-13:05</t>
+        </is>
+      </c>
       <c r="C14" s="1" t="inlineStr">
         <is>
           <t>wło-j2</t>
@@ -17449,7 +17731,11 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n"/>
-      <c r="B17" s="2" t="n"/>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>14:10-14:55</t>
+        </is>
+      </c>
       <c r="C17" s="1" t="inlineStr">
         <is>
           <t>ang-j2</t>
@@ -17549,7 +17835,11 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n"/>
-      <c r="B19" s="2" t="n"/>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>15:00-15:45</t>
+        </is>
+      </c>
       <c r="C19" s="1" t="inlineStr"/>
       <c r="D19" s="1" t="inlineStr"/>
       <c r="E19" s="1" t="inlineStr"/>
@@ -17651,7 +17941,11 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n"/>
-      <c r="B21" s="2" t="n"/>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>15:50-16:35</t>
+        </is>
+      </c>
       <c r="C21" s="1" t="inlineStr"/>
       <c r="D21" s="1" t="inlineStr"/>
       <c r="E21" s="1" t="inlineStr"/>
@@ -17803,28 +18097,20 @@
       <c r="Q23" s="1" t="inlineStr"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="13">
+    <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A18:A19"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
     <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A6:A7"/>
     <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A18:A19"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -18077,7 +18363,11 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n"/>
-      <c r="B5" s="2" t="n"/>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>8:00-8:45</t>
+        </is>
+      </c>
       <c r="C5" s="1" t="inlineStr"/>
       <c r="D5" s="1" t="inlineStr"/>
       <c r="E5" s="1" t="inlineStr"/>
@@ -18175,7 +18465,11 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n"/>
-      <c r="B7" s="2" t="n"/>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>8:50-9:35</t>
+        </is>
+      </c>
       <c r="C7" s="1" t="inlineStr"/>
       <c r="D7" s="1" t="inlineStr"/>
       <c r="E7" s="1" t="inlineStr"/>
@@ -18287,7 +18581,11 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n"/>
-      <c r="B9" s="2" t="n"/>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>9:40-10:25</t>
+        </is>
+      </c>
       <c r="C9" s="1" t="inlineStr"/>
       <c r="D9" s="1" t="inlineStr"/>
       <c r="E9" s="1" t="inlineStr"/>
@@ -18409,7 +18707,11 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n"/>
-      <c r="B11" s="2" t="n"/>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>10:40-11:25</t>
+        </is>
+      </c>
       <c r="C11" s="1" t="inlineStr">
         <is>
           <t>infor-j2</t>
@@ -18537,7 +18839,11 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n"/>
-      <c r="B13" s="2" t="n"/>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>11:30-12:15</t>
+        </is>
+      </c>
       <c r="C13" s="1" t="inlineStr"/>
       <c r="D13" s="1" t="inlineStr"/>
       <c r="E13" s="1" t="inlineStr"/>
@@ -18641,7 +18947,11 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n"/>
-      <c r="B15" s="2" t="n"/>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>12:20-13:05</t>
+        </is>
+      </c>
       <c r="C15" s="1" t="inlineStr">
         <is>
           <t>ang-j2</t>
@@ -18755,7 +19065,11 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n"/>
-      <c r="B17" s="2" t="n"/>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>13:10-13:55</t>
+        </is>
+      </c>
       <c r="C17" s="1" t="inlineStr">
         <is>
           <t>wło-j2</t>
@@ -18873,7 +19187,11 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n"/>
-      <c r="B19" s="2" t="n"/>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>14:10-14:55</t>
+        </is>
+      </c>
       <c r="C19" s="1" t="inlineStr"/>
       <c r="D19" s="1" t="inlineStr"/>
       <c r="E19" s="1" t="inlineStr"/>
@@ -18963,7 +19281,11 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n"/>
-      <c r="B21" s="2" t="n"/>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>15:00-15:45</t>
+        </is>
+      </c>
       <c r="C21" s="1" t="inlineStr"/>
       <c r="D21" s="1" t="inlineStr"/>
       <c r="E21" s="1" t="inlineStr"/>
@@ -19043,7 +19365,11 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n"/>
-      <c r="B23" s="2" t="n"/>
+      <c r="B23" s="2" t="inlineStr">
+        <is>
+          <t>15:50-16:35</t>
+        </is>
+      </c>
       <c r="C23" s="1" t="inlineStr"/>
       <c r="D23" s="1" t="inlineStr"/>
       <c r="E23" s="1" t="inlineStr"/>
@@ -19147,32 +19473,22 @@
       <c r="Q25" s="1" t="inlineStr"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="15">
+    <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="A20:A21"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B16:B17"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -19435,7 +19751,11 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n"/>
-      <c r="B5" s="2" t="n"/>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>8:00-8:45</t>
+        </is>
+      </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
           <t>ang-fry</t>
@@ -19553,7 +19873,11 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n"/>
-      <c r="B7" s="2" t="n"/>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>8:50-9:35</t>
+        </is>
+      </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
           <t>niem-fry</t>
@@ -19675,7 +19999,11 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n"/>
-      <c r="B9" s="2" t="n"/>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>9:40-10:25</t>
+        </is>
+      </c>
       <c r="C9" s="1" t="inlineStr"/>
       <c r="D9" s="1" t="inlineStr"/>
       <c r="E9" s="1" t="inlineStr"/>
@@ -19819,7 +20147,11 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n"/>
-      <c r="B11" s="2" t="n"/>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>10:40-11:25</t>
+        </is>
+      </c>
       <c r="C11" s="1" t="inlineStr"/>
       <c r="D11" s="1" t="inlineStr"/>
       <c r="E11" s="1" t="inlineStr"/>
@@ -19953,7 +20285,11 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n"/>
-      <c r="B13" s="2" t="n"/>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>11:30-12:15</t>
+        </is>
+      </c>
       <c r="C13" s="1" t="inlineStr"/>
       <c r="D13" s="1" t="inlineStr"/>
       <c r="E13" s="1" t="inlineStr"/>
@@ -19996,7 +20332,11 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n"/>
-      <c r="B14" s="2" t="n"/>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>11:30-12:15</t>
+        </is>
+      </c>
       <c r="C14" s="1" t="inlineStr"/>
       <c r="D14" s="1" t="inlineStr"/>
       <c r="E14" s="1" t="inlineStr"/>
@@ -20116,7 +20456,11 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="n"/>
-      <c r="B16" s="2" t="n"/>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>12:20-13:05</t>
+        </is>
+      </c>
       <c r="C16" s="1" t="inlineStr">
         <is>
           <t>w.f-fry</t>
@@ -20171,7 +20515,11 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n"/>
-      <c r="B17" s="2" t="n"/>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>12:20-13:05</t>
+        </is>
+      </c>
       <c r="C17" s="1" t="inlineStr"/>
       <c r="D17" s="1" t="inlineStr"/>
       <c r="E17" s="1" t="inlineStr"/>
@@ -20291,7 +20639,11 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n"/>
-      <c r="B19" s="2" t="n"/>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>13:10-13:55</t>
+        </is>
+      </c>
       <c r="C19" s="1" t="inlineStr"/>
       <c r="D19" s="1" t="inlineStr"/>
       <c r="E19" s="1" t="inlineStr"/>
@@ -20409,7 +20761,11 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n"/>
-      <c r="B21" s="2" t="n"/>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>14:10-14:55</t>
+        </is>
+      </c>
       <c r="C21" s="1" t="inlineStr"/>
       <c r="D21" s="1" t="inlineStr"/>
       <c r="E21" s="1" t="inlineStr"/>
@@ -20590,28 +20946,20 @@
       <c r="Q24" s="1" t="inlineStr"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="13">
+    <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="A8:A9"/>
     <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B4:B5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>